<commit_message>
upload utility template updated
Signed-off-by: Sahoo Himansu <himansu.sahoo1986@gmail.com>
</commit_message>
<xml_diff>
--- a/uploads/upload_templates/book_ledger_batch_upload_template.xlsx
+++ b/uploads/upload_templates/book_ledger_batch_upload_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\xampp\htdocs\projects\chm\uploads\upload_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BBACAC-FC0F-4C0D-BA11-730F96C2D820}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE82316-7D05-4F2D-888C-D6B4A59C71B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upload_data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>BOOK_NAME</t>
   </si>
@@ -67,13 +67,19 @@
   </si>
   <si>
     <t>PURCHASE_REMARKS</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +91,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,9 +160,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,54 +462,100 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>